<commit_message>
Area chart, absolute profit.
</commit_message>
<xml_diff>
--- a/msci-world-index-historical-data-1969-2018.xlsx
+++ b/msci-world-index-historical-data-1969-2018.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mikael Ahonen\OneDrive\Projektit\2018-12-02 Sijoituksen ajoittaminen\economical-cycle-timing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3ad052d390b60130/Projektit/2018-12-02 Sijoituksen ajoittaminen/economical-cycle-timing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C9F7CB3-3F7B-4992-8BC0-BED8043F093D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="102_{12D0ACAF-1BF2-49E4-B106-D1A9D18721E2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{3B5065FD-3014-4925-A281-CC5CAF1904C8}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1800" windowWidth="28800" windowHeight="12150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2400" windowWidth="28800" windowHeight="12150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
     <t>date</t>
   </si>
   <si>
-    <t>value</t>
+    <t>price</t>
   </si>
 </sst>
 </file>
@@ -266,7 +266,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>value</c:v>
+                  <c:v>price</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4622,7 +4622,7 @@
   <autoFilter ref="A1:B589" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="date" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="value" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="price" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4927,7 +4927,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B589"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Create mp4 video from charts.
</commit_message>
<xml_diff>
--- a/msci-world-index-historical-data-1969-2018.xlsx
+++ b/msci-world-index-historical-data-1969-2018.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3ad052d390b60130/Projektit/2018-12-02 Sijoituksen ajoittaminen/economical-cycle-timing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mikael Ahonen\OneDrive\Projektit\2018-12-02 Sijoituksen ajoittaminen\economical-cycle-timing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="102_{12D0ACAF-1BF2-49E4-B106-D1A9D18721E2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{3B5065FD-3014-4925-A281-CC5CAF1904C8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8191F59A-3AAE-49DF-B60E-EFC1EF139D05}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2400" windowWidth="28800" windowHeight="12150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3000" windowWidth="28800" windowHeight="12150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -222,6 +222,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>MSCI World Index</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4577,7 +4602,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="121" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="114" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4588,7 +4613,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9304587" cy="6077107"/>
+    <xdr:ext cx="9301370" cy="6071152"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Kaavio 1">
@@ -4927,13 +4952,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B589"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>